<commit_message>
Atualizacao regulares e irregulares
</commit_message>
<xml_diff>
--- a/pacientes_irregulares.xlsx
+++ b/pacientes_irregulares.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="81">
   <si>
     <t>CO_PA_CNSPAC</t>
   </si>
@@ -28,21 +28,21 @@
     <t>CO_PA_CMP_biopsia</t>
   </si>
   <si>
+    <t>CO_PA_PROC_ID_anatomo</t>
+  </si>
+  <si>
+    <t>CO_PA_MVM_anatomo</t>
+  </si>
+  <si>
+    <t>CO_PA_CMP_anatomo</t>
+  </si>
+  <si>
     <t>NU_PA_QTDAPR_biopsia</t>
   </si>
   <si>
     <t>NU_PA_VALAPR_biopsia</t>
   </si>
   <si>
-    <t>CO_PA_PROC_ID_anatomo</t>
-  </si>
-  <si>
-    <t>CO_PA_MVM_anatomo</t>
-  </si>
-  <si>
-    <t>CO_PA_CMP_anatomo</t>
-  </si>
-  <si>
     <t>NU_PA_QTDAPR_anatomo</t>
   </si>
   <si>
@@ -58,6 +58,9 @@
     <t>209788669530007</t>
   </si>
   <si>
+    <t>700003763941309</t>
+  </si>
+  <si>
     <t>700203453089521</t>
   </si>
   <si>
@@ -250,28 +253,10 @@
     <t>202305</t>
   </si>
   <si>
-    <t>202,81</t>
-  </si>
-  <si>
-    <t>202,81202,81</t>
-  </si>
-  <si>
     <t>0203020030</t>
   </si>
   <si>
     <t>202309</t>
-  </si>
-  <si>
-    <t>244,68</t>
-  </si>
-  <si>
-    <t>40,7840,78</t>
-  </si>
-  <si>
-    <t>285,46</t>
-  </si>
-  <si>
-    <t>203,9</t>
   </si>
 </sst>
 </file>
@@ -629,7 +614,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -675,34 +660,34 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D2">
         <v>202310</v>
       </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="E2" t="s">
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H2" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G2">
+        <v>202310</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J2">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
-        <v>82</v>
+      <c r="K2">
+        <v>244.68</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -710,34 +695,34 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D3">
         <v>202310</v>
       </c>
-      <c r="E3">
-        <v>1</v>
+      <c r="E3" t="s">
+        <v>79</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G3">
+        <v>202310</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J3">
         <v>6</v>
       </c>
-      <c r="K3" t="s">
-        <v>82</v>
+      <c r="K3">
+        <v>244.68</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -745,34 +730,34 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D4">
         <v>202310</v>
       </c>
-      <c r="E4">
-        <v>1</v>
+      <c r="E4" t="s">
+        <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G4">
+        <v>202310</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J4">
         <v>6</v>
       </c>
-      <c r="K4" t="s">
-        <v>82</v>
+      <c r="K4">
+        <v>244.68</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -780,34 +765,34 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D5">
-        <v>202310</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
+        <v>202306</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="G5">
+        <v>202306</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>202310</v>
+        <v>405.62</v>
       </c>
       <c r="J5">
-        <v>6</v>
-      </c>
-      <c r="K5" t="s">
-        <v>82</v>
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>40.78</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -815,34 +800,34 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
         <v>72</v>
       </c>
       <c r="D6">
-        <v>202306</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E6" t="s">
+        <v>79</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G6" t="s">
-        <v>80</v>
-      </c>
-      <c r="H6" t="s">
-        <v>81</v>
+        <v>72</v>
+      </c>
+      <c r="G6">
+        <v>202310</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>202309</v>
+        <v>202.81</v>
       </c>
       <c r="J6">
-        <v>2</v>
-      </c>
-      <c r="K6" t="s">
-        <v>83</v>
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <v>244.68</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -850,34 +835,34 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D7">
-        <v>202310</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
+        <v>202306</v>
+      </c>
+      <c r="E7" t="s">
+        <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" t="s">
         <v>80</v>
       </c>
-      <c r="H7" t="s">
-        <v>71</v>
+      <c r="G7">
+        <v>202309</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J7">
-        <v>6</v>
-      </c>
-      <c r="K7" t="s">
-        <v>82</v>
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>81.56</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -885,34 +870,34 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D8">
-        <v>202309</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E8" t="s">
+        <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="G8">
+        <v>202310</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>202302</v>
+        <v>202.81</v>
       </c>
       <c r="J8">
         <v>6</v>
       </c>
-      <c r="K8" t="s">
-        <v>82</v>
+      <c r="K8">
+        <v>244.68</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -920,34 +905,34 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D9">
-        <v>202310</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
+        <v>202309</v>
+      </c>
+      <c r="E9" t="s">
+        <v>79</v>
       </c>
       <c r="F9" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H9" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="G9">
+        <v>202302</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J9">
-        <v>7</v>
-      </c>
-      <c r="K9" t="s">
-        <v>84</v>
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>244.68</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -955,34 +940,34 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D10">
         <v>202310</v>
       </c>
-      <c r="E10">
-        <v>1</v>
+      <c r="E10" t="s">
+        <v>79</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G10">
+        <v>202310</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J10">
-        <v>6</v>
-      </c>
-      <c r="K10" t="s">
-        <v>82</v>
+        <v>7</v>
+      </c>
+      <c r="K10">
+        <v>285.46</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -990,34 +975,34 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>202310</v>
       </c>
-      <c r="E11">
-        <v>1</v>
+      <c r="E11" t="s">
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H11" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G11">
+        <v>202310</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J11">
         <v>6</v>
       </c>
-      <c r="K11" t="s">
-        <v>82</v>
+      <c r="K11">
+        <v>244.68</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1025,34 +1010,34 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D12">
         <v>202310</v>
       </c>
-      <c r="E12">
-        <v>1</v>
+      <c r="E12" t="s">
+        <v>79</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
-      </c>
-      <c r="G12" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G12">
+        <v>202310</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J12">
         <v>6</v>
       </c>
-      <c r="K12" t="s">
-        <v>82</v>
+      <c r="K12">
+        <v>244.68</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1060,34 +1045,34 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13">
-        <v>202303</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" t="s">
-        <v>80</v>
-      </c>
-      <c r="H13" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="G13">
+        <v>202310</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>202303</v>
+        <v>202.81</v>
       </c>
       <c r="J13">
         <v>6</v>
       </c>
-      <c r="K13" t="s">
-        <v>82</v>
+      <c r="K13">
+        <v>244.68</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1095,34 +1080,34 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D14">
         <v>202303</v>
       </c>
-      <c r="E14">
-        <v>1</v>
+      <c r="E14" t="s">
+        <v>79</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H14" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="G14">
+        <v>202303</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>202303</v>
+        <v>202.81</v>
       </c>
       <c r="J14">
-        <v>5</v>
-      </c>
-      <c r="K14" t="s">
-        <v>85</v>
+        <v>6</v>
+      </c>
+      <c r="K14">
+        <v>244.68</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1130,34 +1115,34 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D15">
-        <v>202310</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
+        <v>202303</v>
+      </c>
+      <c r="E15" t="s">
+        <v>79</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="G15">
+        <v>202303</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J15">
-        <v>6</v>
-      </c>
-      <c r="K15" t="s">
-        <v>82</v>
+        <v>5</v>
+      </c>
+      <c r="K15">
+        <v>203.9</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1165,34 +1150,34 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D16">
-        <v>202302</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E16" t="s">
+        <v>79</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
-      </c>
-      <c r="G16" t="s">
-        <v>80</v>
-      </c>
-      <c r="H16" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="G16">
+        <v>202310</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
       </c>
       <c r="I16">
-        <v>202302</v>
+        <v>202.81</v>
       </c>
       <c r="J16">
         <v>6</v>
       </c>
-      <c r="K16" t="s">
-        <v>82</v>
+      <c r="K16">
+        <v>244.68</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1200,34 +1185,34 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D17">
-        <v>202310</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
+        <v>202302</v>
+      </c>
+      <c r="E17" t="s">
+        <v>79</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="G17">
+        <v>202302</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J17">
         <v>6</v>
       </c>
-      <c r="K17" t="s">
-        <v>82</v>
+      <c r="K17">
+        <v>244.68</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1235,34 +1220,34 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18">
-        <v>202303</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E18" t="s">
+        <v>79</v>
       </c>
       <c r="F18" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" t="s">
-        <v>80</v>
-      </c>
-      <c r="H18" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="G18">
+        <v>202310</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
       </c>
       <c r="I18">
-        <v>202303</v>
+        <v>202.81</v>
       </c>
       <c r="J18">
         <v>6</v>
       </c>
-      <c r="K18" t="s">
-        <v>82</v>
+      <c r="K18">
+        <v>244.68</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1270,34 +1255,34 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D19">
-        <v>202310</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
+        <v>202303</v>
+      </c>
+      <c r="E19" t="s">
+        <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" t="s">
-        <v>80</v>
-      </c>
-      <c r="H19" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="G19">
+        <v>202303</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J19">
         <v>6</v>
       </c>
-      <c r="K19" t="s">
-        <v>82</v>
+      <c r="K19">
+        <v>244.68</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1305,34 +1290,34 @@
         <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D20">
-        <v>202304</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
+        <v>202310</v>
+      </c>
+      <c r="E20" t="s">
+        <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" t="s">
-        <v>80</v>
-      </c>
-      <c r="H20" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+      <c r="G20">
+        <v>202310</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>202304</v>
+        <v>202.81</v>
       </c>
       <c r="J20">
-        <v>2</v>
-      </c>
-      <c r="K20" t="s">
-        <v>83</v>
+        <v>6</v>
+      </c>
+      <c r="K20">
+        <v>244.68</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1340,34 +1325,34 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D21">
-        <v>202310</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
+        <v>202304</v>
+      </c>
+      <c r="E21" t="s">
+        <v>79</v>
       </c>
       <c r="F21" t="s">
-        <v>78</v>
-      </c>
-      <c r="G21" t="s">
-        <v>80</v>
-      </c>
-      <c r="H21" t="s">
-        <v>71</v>
+        <v>76</v>
+      </c>
+      <c r="G21">
+        <v>202304</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
       </c>
       <c r="I21">
-        <v>202310</v>
+        <v>405.62</v>
       </c>
       <c r="J21">
-        <v>7</v>
-      </c>
-      <c r="K21" t="s">
-        <v>84</v>
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <v>81.56</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1375,34 +1360,34 @@
         <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D22">
-        <v>202301</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E22" t="s">
+        <v>79</v>
       </c>
       <c r="F22" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" t="s">
-        <v>80</v>
-      </c>
-      <c r="H22" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="G22">
+        <v>202310</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>202302</v>
+        <v>202.81</v>
       </c>
       <c r="J22">
-        <v>6</v>
-      </c>
-      <c r="K22" t="s">
-        <v>82</v>
+        <v>7</v>
+      </c>
+      <c r="K22">
+        <v>285.46</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1410,34 +1395,34 @@
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D23">
-        <v>202310</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
+        <v>202301</v>
+      </c>
+      <c r="E23" t="s">
+        <v>79</v>
       </c>
       <c r="F23" t="s">
-        <v>78</v>
-      </c>
-      <c r="G23" t="s">
-        <v>80</v>
-      </c>
-      <c r="H23" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="G23">
+        <v>202302</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J23">
         <v>6</v>
       </c>
-      <c r="K23" t="s">
-        <v>82</v>
+      <c r="K23">
+        <v>244.68</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1445,34 +1430,34 @@
         <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D24">
-        <v>202304</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E24" t="s">
+        <v>79</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24" t="s">
-        <v>80</v>
-      </c>
-      <c r="H24" t="s">
-        <v>75</v>
+        <v>72</v>
+      </c>
+      <c r="G24">
+        <v>202310</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>202304</v>
+        <v>202.81</v>
       </c>
       <c r="J24">
         <v>6</v>
       </c>
-      <c r="K24" t="s">
-        <v>82</v>
+      <c r="K24">
+        <v>244.68</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1480,34 +1465,34 @@
         <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D25">
-        <v>202310</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
+        <v>202304</v>
+      </c>
+      <c r="E25" t="s">
+        <v>79</v>
       </c>
       <c r="F25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G25" t="s">
-        <v>80</v>
-      </c>
-      <c r="H25" t="s">
-        <v>71</v>
+        <v>76</v>
+      </c>
+      <c r="G25">
+        <v>202304</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J25">
         <v>6</v>
       </c>
-      <c r="K25" t="s">
-        <v>82</v>
+      <c r="K25">
+        <v>244.68</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1515,34 +1500,34 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D26">
-        <v>202302</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E26" t="s">
+        <v>79</v>
       </c>
       <c r="F26" t="s">
-        <v>78</v>
-      </c>
-      <c r="G26" t="s">
-        <v>80</v>
-      </c>
-      <c r="H26" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="G26">
+        <v>202310</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
       </c>
       <c r="I26">
-        <v>202302</v>
+        <v>202.81</v>
       </c>
       <c r="J26">
         <v>6</v>
       </c>
-      <c r="K26" t="s">
-        <v>82</v>
+      <c r="K26">
+        <v>244.68</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1550,34 +1535,34 @@
         <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D27">
         <v>202302</v>
       </c>
-      <c r="E27">
-        <v>1</v>
+      <c r="E27" t="s">
+        <v>79</v>
       </c>
       <c r="F27" t="s">
-        <v>78</v>
-      </c>
-      <c r="G27" t="s">
-        <v>80</v>
-      </c>
-      <c r="H27" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="G27">
+        <v>202302</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
       </c>
       <c r="I27">
-        <v>202303</v>
+        <v>202.81</v>
       </c>
       <c r="J27">
         <v>6</v>
       </c>
-      <c r="K27" t="s">
-        <v>82</v>
+      <c r="K27">
+        <v>244.68</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1585,34 +1570,34 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D28">
-        <v>202304</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
+        <v>202302</v>
+      </c>
+      <c r="E28" t="s">
+        <v>79</v>
       </c>
       <c r="F28" t="s">
-        <v>78</v>
-      </c>
-      <c r="G28" t="s">
-        <v>80</v>
-      </c>
-      <c r="H28" t="s">
         <v>74</v>
       </c>
+      <c r="G28">
+        <v>202303</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
       <c r="I28">
-        <v>202302</v>
+        <v>202.81</v>
       </c>
       <c r="J28">
-        <v>2</v>
-      </c>
-      <c r="K28" t="s">
-        <v>83</v>
+        <v>6</v>
+      </c>
+      <c r="K28">
+        <v>244.68</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1620,34 +1605,34 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D29">
-        <v>202303</v>
-      </c>
-      <c r="E29">
+        <v>202304</v>
+      </c>
+      <c r="E29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29">
+        <v>202302</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>202.81</v>
+      </c>
+      <c r="J29">
         <v>2</v>
       </c>
-      <c r="F29" t="s">
-        <v>79</v>
-      </c>
-      <c r="G29" t="s">
-        <v>80</v>
-      </c>
-      <c r="H29" t="s">
-        <v>75</v>
-      </c>
-      <c r="I29">
-        <v>202304</v>
-      </c>
-      <c r="J29">
-        <v>6</v>
-      </c>
-      <c r="K29" t="s">
-        <v>82</v>
+      <c r="K29">
+        <v>81.56</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1655,34 +1640,34 @@
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D30">
-        <v>202310</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
+        <v>202303</v>
+      </c>
+      <c r="E30" t="s">
+        <v>79</v>
       </c>
       <c r="F30" t="s">
-        <v>78</v>
-      </c>
-      <c r="G30" t="s">
-        <v>80</v>
-      </c>
-      <c r="H30" t="s">
         <v>76</v>
       </c>
+      <c r="G30">
+        <v>202304</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
       <c r="I30">
-        <v>202301</v>
+        <v>405.62</v>
       </c>
       <c r="J30">
         <v>6</v>
       </c>
-      <c r="K30" t="s">
-        <v>82</v>
+      <c r="K30">
+        <v>244.68</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1690,69 +1675,69 @@
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D31">
-        <v>202302</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E31" t="s">
+        <v>79</v>
       </c>
       <c r="F31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" t="s">
-        <v>80</v>
-      </c>
-      <c r="H31" t="s">
-        <v>74</v>
+        <v>77</v>
+      </c>
+      <c r="G31">
+        <v>202301</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
       </c>
       <c r="I31">
-        <v>202302</v>
+        <v>202.81</v>
       </c>
       <c r="J31">
         <v>6</v>
       </c>
-      <c r="K31" t="s">
-        <v>82</v>
+      <c r="K31">
+        <v>244.68</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D32">
-        <v>202310</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
+        <v>202302</v>
+      </c>
+      <c r="E32" t="s">
+        <v>79</v>
       </c>
       <c r="F32" t="s">
-        <v>78</v>
-      </c>
-      <c r="G32" t="s">
-        <v>80</v>
-      </c>
-      <c r="H32" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="G32">
+        <v>202302</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
       </c>
       <c r="I32">
-        <v>202302</v>
+        <v>202.81</v>
       </c>
       <c r="J32">
         <v>6</v>
       </c>
-      <c r="K32" t="s">
-        <v>82</v>
+      <c r="K32">
+        <v>244.68</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1760,34 +1745,34 @@
         <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D33">
         <v>202310</v>
       </c>
-      <c r="E33">
-        <v>1</v>
+      <c r="E33" t="s">
+        <v>79</v>
       </c>
       <c r="F33" t="s">
-        <v>78</v>
-      </c>
-      <c r="G33" t="s">
-        <v>80</v>
-      </c>
-      <c r="H33" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="G33">
+        <v>202302</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J33">
         <v>6</v>
       </c>
-      <c r="K33" t="s">
-        <v>82</v>
+      <c r="K33">
+        <v>244.68</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1795,69 +1780,69 @@
         <v>42</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D34">
-        <v>202301</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E34" t="s">
+        <v>79</v>
       </c>
       <c r="F34" t="s">
-        <v>78</v>
-      </c>
-      <c r="G34" t="s">
-        <v>80</v>
-      </c>
-      <c r="H34" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="G34">
+        <v>202310</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
       </c>
       <c r="I34">
-        <v>202302</v>
+        <v>202.81</v>
       </c>
       <c r="J34">
         <v>6</v>
       </c>
-      <c r="K34" t="s">
-        <v>82</v>
+      <c r="K34">
+        <v>244.68</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D35">
-        <v>202303</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
+        <v>202301</v>
+      </c>
+      <c r="E35" t="s">
+        <v>79</v>
       </c>
       <c r="F35" t="s">
-        <v>78</v>
-      </c>
-      <c r="G35" t="s">
-        <v>80</v>
-      </c>
-      <c r="H35" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="G35">
+        <v>202302</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
       </c>
       <c r="I35">
-        <v>202302</v>
+        <v>202.81</v>
       </c>
       <c r="J35">
         <v>6</v>
       </c>
-      <c r="K35" t="s">
-        <v>82</v>
+      <c r="K35">
+        <v>244.68</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1865,34 +1850,34 @@
         <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D36">
-        <v>202310</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
+        <v>202303</v>
+      </c>
+      <c r="E36" t="s">
+        <v>79</v>
       </c>
       <c r="F36" t="s">
-        <v>78</v>
-      </c>
-      <c r="G36" t="s">
-        <v>80</v>
-      </c>
-      <c r="H36" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="G36">
+        <v>202302</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
       </c>
       <c r="I36">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J36">
         <v>6</v>
       </c>
-      <c r="K36" t="s">
-        <v>82</v>
+      <c r="K36">
+        <v>244.68</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -1900,34 +1885,34 @@
         <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D37">
         <v>202310</v>
       </c>
-      <c r="E37">
-        <v>1</v>
+      <c r="E37" t="s">
+        <v>79</v>
       </c>
       <c r="F37" t="s">
-        <v>78</v>
-      </c>
-      <c r="G37" t="s">
-        <v>80</v>
-      </c>
-      <c r="H37" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G37">
+        <v>202310</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
       </c>
       <c r="I37">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J37">
         <v>6</v>
       </c>
-      <c r="K37" t="s">
-        <v>82</v>
+      <c r="K37">
+        <v>244.68</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1935,34 +1920,34 @@
         <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D38">
         <v>202310</v>
       </c>
-      <c r="E38">
-        <v>1</v>
+      <c r="E38" t="s">
+        <v>79</v>
       </c>
       <c r="F38" t="s">
-        <v>78</v>
-      </c>
-      <c r="G38" t="s">
-        <v>80</v>
-      </c>
-      <c r="H38" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G38">
+        <v>202310</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
       </c>
       <c r="I38">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J38">
         <v>6</v>
       </c>
-      <c r="K38" t="s">
-        <v>82</v>
+      <c r="K38">
+        <v>244.68</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1970,34 +1955,34 @@
         <v>46</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D39">
         <v>202310</v>
       </c>
-      <c r="E39">
-        <v>1</v>
+      <c r="E39" t="s">
+        <v>79</v>
       </c>
       <c r="F39" t="s">
-        <v>78</v>
-      </c>
-      <c r="G39" t="s">
-        <v>80</v>
-      </c>
-      <c r="H39" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G39">
+        <v>202310</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
       </c>
       <c r="I39">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J39">
         <v>6</v>
       </c>
-      <c r="K39" t="s">
-        <v>82</v>
+      <c r="K39">
+        <v>244.68</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -2005,34 +1990,34 @@
         <v>47</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D40">
         <v>202310</v>
       </c>
-      <c r="E40">
-        <v>1</v>
+      <c r="E40" t="s">
+        <v>79</v>
       </c>
       <c r="F40" t="s">
-        <v>78</v>
-      </c>
-      <c r="G40" t="s">
-        <v>80</v>
-      </c>
-      <c r="H40" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G40">
+        <v>202310</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
       </c>
       <c r="I40">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J40">
-        <v>7</v>
-      </c>
-      <c r="K40" t="s">
-        <v>84</v>
+        <v>6</v>
+      </c>
+      <c r="K40">
+        <v>244.68</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2040,34 +2025,34 @@
         <v>48</v>
       </c>
       <c r="B41" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D41">
         <v>202310</v>
       </c>
-      <c r="E41">
-        <v>1</v>
+      <c r="E41" t="s">
+        <v>79</v>
       </c>
       <c r="F41" t="s">
-        <v>78</v>
-      </c>
-      <c r="G41" t="s">
-        <v>80</v>
-      </c>
-      <c r="H41" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G41">
+        <v>202310</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
       </c>
       <c r="I41">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J41">
-        <v>6</v>
-      </c>
-      <c r="K41" t="s">
-        <v>82</v>
+        <v>7</v>
+      </c>
+      <c r="K41">
+        <v>285.46</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2075,34 +2060,34 @@
         <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D42">
         <v>202310</v>
       </c>
-      <c r="E42">
-        <v>1</v>
+      <c r="E42" t="s">
+        <v>79</v>
       </c>
       <c r="F42" t="s">
-        <v>78</v>
-      </c>
-      <c r="G42" t="s">
-        <v>80</v>
-      </c>
-      <c r="H42" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G42">
+        <v>202310</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J42">
         <v>6</v>
       </c>
-      <c r="K42" t="s">
-        <v>82</v>
+      <c r="K42">
+        <v>244.68</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2110,34 +2095,34 @@
         <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D43">
         <v>202310</v>
       </c>
-      <c r="E43">
-        <v>1</v>
+      <c r="E43" t="s">
+        <v>79</v>
       </c>
       <c r="F43" t="s">
-        <v>78</v>
-      </c>
-      <c r="G43" t="s">
-        <v>80</v>
-      </c>
-      <c r="H43" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G43">
+        <v>202310</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
       </c>
       <c r="I43">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J43">
         <v>6</v>
       </c>
-      <c r="K43" t="s">
-        <v>82</v>
+      <c r="K43">
+        <v>244.68</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2145,34 +2130,34 @@
         <v>51</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C44" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D44">
         <v>202310</v>
       </c>
-      <c r="E44">
-        <v>1</v>
+      <c r="E44" t="s">
+        <v>79</v>
       </c>
       <c r="F44" t="s">
-        <v>78</v>
-      </c>
-      <c r="G44" t="s">
-        <v>80</v>
-      </c>
-      <c r="H44" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G44">
+        <v>202310</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
       </c>
       <c r="I44">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J44">
         <v>6</v>
       </c>
-      <c r="K44" t="s">
-        <v>82</v>
+      <c r="K44">
+        <v>244.68</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2180,34 +2165,34 @@
         <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D45">
-        <v>202301</v>
-      </c>
-      <c r="E45">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E45" t="s">
+        <v>79</v>
       </c>
       <c r="F45" t="s">
-        <v>78</v>
-      </c>
-      <c r="G45" t="s">
-        <v>80</v>
-      </c>
-      <c r="H45" t="s">
-        <v>72</v>
+        <v>72</v>
+      </c>
+      <c r="G45">
+        <v>202310</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
       </c>
       <c r="I45">
-        <v>202304</v>
+        <v>202.81</v>
       </c>
       <c r="J45">
         <v>6</v>
       </c>
-      <c r="K45" t="s">
-        <v>82</v>
+      <c r="K45">
+        <v>244.68</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2215,34 +2200,34 @@
         <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C46" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46">
+        <v>202301</v>
+      </c>
+      <c r="E46" t="s">
+        <v>79</v>
+      </c>
+      <c r="F46" t="s">
         <v>73</v>
       </c>
-      <c r="D46">
-        <v>202303</v>
-      </c>
-      <c r="E46">
-        <v>1</v>
-      </c>
-      <c r="F46" t="s">
-        <v>78</v>
-      </c>
-      <c r="G46" t="s">
-        <v>80</v>
-      </c>
-      <c r="H46" t="s">
-        <v>73</v>
+      <c r="G46">
+        <v>202304</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
       </c>
       <c r="I46">
-        <v>202303</v>
+        <v>202.81</v>
       </c>
       <c r="J46">
         <v>6</v>
       </c>
-      <c r="K46" t="s">
-        <v>82</v>
+      <c r="K46">
+        <v>244.68</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2250,34 +2235,34 @@
         <v>54</v>
       </c>
       <c r="B47" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C47" t="s">
         <v>74</v>
       </c>
       <c r="D47">
-        <v>202302</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
+        <v>202303</v>
+      </c>
+      <c r="E47" t="s">
+        <v>79</v>
       </c>
       <c r="F47" t="s">
-        <v>78</v>
-      </c>
-      <c r="G47" t="s">
-        <v>80</v>
-      </c>
-      <c r="H47" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="G47">
+        <v>202303</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
       </c>
       <c r="I47">
-        <v>202303</v>
+        <v>202.81</v>
       </c>
       <c r="J47">
         <v>6</v>
       </c>
-      <c r="K47" t="s">
-        <v>82</v>
+      <c r="K47">
+        <v>244.68</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2285,34 +2270,34 @@
         <v>55</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C48" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D48">
-        <v>202310</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
+        <v>202302</v>
+      </c>
+      <c r="E48" t="s">
+        <v>79</v>
       </c>
       <c r="F48" t="s">
-        <v>78</v>
-      </c>
-      <c r="G48" t="s">
-        <v>80</v>
-      </c>
-      <c r="H48" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="G48">
+        <v>202303</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
       </c>
       <c r="I48">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J48">
         <v>6</v>
       </c>
-      <c r="K48" t="s">
-        <v>82</v>
+      <c r="K48">
+        <v>244.68</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2320,34 +2305,34 @@
         <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D49">
-        <v>202302</v>
-      </c>
-      <c r="E49">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E49" t="s">
+        <v>79</v>
       </c>
       <c r="F49" t="s">
-        <v>78</v>
-      </c>
-      <c r="G49" t="s">
-        <v>80</v>
-      </c>
-      <c r="H49" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="G49">
+        <v>202310</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
       </c>
       <c r="I49">
-        <v>202302</v>
+        <v>202.81</v>
       </c>
       <c r="J49">
-        <v>7</v>
-      </c>
-      <c r="K49" t="s">
-        <v>84</v>
+        <v>6</v>
+      </c>
+      <c r="K49">
+        <v>244.68</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2355,34 +2340,34 @@
         <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D50">
-        <v>202310</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
+        <v>202302</v>
+      </c>
+      <c r="E50" t="s">
+        <v>79</v>
       </c>
       <c r="F50" t="s">
-        <v>78</v>
-      </c>
-      <c r="G50" t="s">
-        <v>80</v>
-      </c>
-      <c r="H50" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="G50">
+        <v>202302</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
       </c>
       <c r="I50">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J50">
-        <v>6</v>
-      </c>
-      <c r="K50" t="s">
-        <v>82</v>
+        <v>7</v>
+      </c>
+      <c r="K50">
+        <v>285.46</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2390,34 +2375,34 @@
         <v>58</v>
       </c>
       <c r="B51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D51">
-        <v>202302</v>
-      </c>
-      <c r="E51">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E51" t="s">
+        <v>79</v>
       </c>
       <c r="F51" t="s">
-        <v>78</v>
-      </c>
-      <c r="G51" t="s">
-        <v>80</v>
-      </c>
-      <c r="H51" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="G51">
+        <v>202310</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
       </c>
       <c r="I51">
-        <v>202303</v>
+        <v>202.81</v>
       </c>
       <c r="J51">
         <v>6</v>
       </c>
-      <c r="K51" t="s">
-        <v>82</v>
+      <c r="K51">
+        <v>244.68</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2425,34 +2410,34 @@
         <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C52" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D52">
-        <v>202310</v>
-      </c>
-      <c r="E52">
-        <v>1</v>
+        <v>202302</v>
+      </c>
+      <c r="E52" t="s">
+        <v>79</v>
       </c>
       <c r="F52" t="s">
-        <v>78</v>
-      </c>
-      <c r="G52" t="s">
-        <v>80</v>
-      </c>
-      <c r="H52" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="G52">
+        <v>202303</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
       </c>
       <c r="I52">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J52">
         <v>6</v>
       </c>
-      <c r="K52" t="s">
-        <v>82</v>
+      <c r="K52">
+        <v>244.68</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2460,34 +2445,34 @@
         <v>60</v>
       </c>
       <c r="B53" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C53" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D53">
-        <v>202302</v>
-      </c>
-      <c r="E53">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E53" t="s">
+        <v>79</v>
       </c>
       <c r="F53" t="s">
-        <v>78</v>
-      </c>
-      <c r="G53" t="s">
-        <v>80</v>
-      </c>
-      <c r="H53" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="G53">
+        <v>202310</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
       </c>
       <c r="I53">
-        <v>202303</v>
+        <v>202.81</v>
       </c>
       <c r="J53">
         <v>6</v>
       </c>
-      <c r="K53" t="s">
-        <v>82</v>
+      <c r="K53">
+        <v>244.68</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2495,34 +2480,34 @@
         <v>61</v>
       </c>
       <c r="B54" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C54" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D54">
-        <v>202310</v>
-      </c>
-      <c r="E54">
-        <v>1</v>
+        <v>202302</v>
+      </c>
+      <c r="E54" t="s">
+        <v>79</v>
       </c>
       <c r="F54" t="s">
-        <v>78</v>
-      </c>
-      <c r="G54" t="s">
-        <v>80</v>
-      </c>
-      <c r="H54" t="s">
-        <v>71</v>
+        <v>74</v>
+      </c>
+      <c r="G54">
+        <v>202303</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
       </c>
       <c r="I54">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J54">
         <v>6</v>
       </c>
-      <c r="K54" t="s">
-        <v>82</v>
+      <c r="K54">
+        <v>244.68</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2530,34 +2515,34 @@
         <v>62</v>
       </c>
       <c r="B55" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C55" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D55">
-        <v>202302</v>
-      </c>
-      <c r="E55">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E55" t="s">
+        <v>79</v>
       </c>
       <c r="F55" t="s">
-        <v>78</v>
-      </c>
-      <c r="G55" t="s">
-        <v>80</v>
-      </c>
-      <c r="H55" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="G55">
+        <v>202310</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
       </c>
       <c r="I55">
-        <v>202302</v>
+        <v>202.81</v>
       </c>
       <c r="J55">
-        <v>7</v>
-      </c>
-      <c r="K55" t="s">
-        <v>84</v>
+        <v>6</v>
+      </c>
+      <c r="K55">
+        <v>244.68</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -2565,34 +2550,34 @@
         <v>63</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D56">
-        <v>202310</v>
-      </c>
-      <c r="E56">
-        <v>1</v>
+        <v>202302</v>
+      </c>
+      <c r="E56" t="s">
+        <v>79</v>
       </c>
       <c r="F56" t="s">
-        <v>78</v>
-      </c>
-      <c r="G56" t="s">
-        <v>80</v>
-      </c>
-      <c r="H56" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="G56">
+        <v>202302</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
       </c>
       <c r="I56">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J56">
-        <v>6</v>
-      </c>
-      <c r="K56" t="s">
-        <v>82</v>
+        <v>7</v>
+      </c>
+      <c r="K56">
+        <v>285.46</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -2600,34 +2585,34 @@
         <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C57" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D57">
         <v>202310</v>
       </c>
-      <c r="E57">
-        <v>1</v>
+      <c r="E57" t="s">
+        <v>79</v>
       </c>
       <c r="F57" t="s">
-        <v>78</v>
-      </c>
-      <c r="G57" t="s">
-        <v>80</v>
-      </c>
-      <c r="H57" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G57">
+        <v>202310</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
       </c>
       <c r="I57">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J57">
         <v>6</v>
       </c>
-      <c r="K57" t="s">
-        <v>82</v>
+      <c r="K57">
+        <v>244.68</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -2635,34 +2620,34 @@
         <v>65</v>
       </c>
       <c r="B58" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D58">
         <v>202310</v>
       </c>
-      <c r="E58">
-        <v>1</v>
+      <c r="E58" t="s">
+        <v>79</v>
       </c>
       <c r="F58" t="s">
-        <v>78</v>
-      </c>
-      <c r="G58" t="s">
-        <v>80</v>
-      </c>
-      <c r="H58" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G58">
+        <v>202310</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
       </c>
       <c r="I58">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J58">
         <v>6</v>
       </c>
-      <c r="K58" t="s">
-        <v>82</v>
+      <c r="K58">
+        <v>244.68</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -2670,34 +2655,34 @@
         <v>66</v>
       </c>
       <c r="B59" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C59" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D59">
         <v>202310</v>
       </c>
-      <c r="E59">
-        <v>1</v>
+      <c r="E59" t="s">
+        <v>79</v>
       </c>
       <c r="F59" t="s">
-        <v>78</v>
-      </c>
-      <c r="G59" t="s">
-        <v>80</v>
-      </c>
-      <c r="H59" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="G59">
+        <v>202310</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
       </c>
       <c r="I59">
-        <v>202310</v>
+        <v>202.81</v>
       </c>
       <c r="J59">
         <v>6</v>
       </c>
-      <c r="K59" t="s">
-        <v>82</v>
+      <c r="K59">
+        <v>244.68</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -2705,34 +2690,34 @@
         <v>67</v>
       </c>
       <c r="B60" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C60" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D60">
-        <v>202302</v>
-      </c>
-      <c r="E60">
-        <v>1</v>
+        <v>202310</v>
+      </c>
+      <c r="E60" t="s">
+        <v>79</v>
       </c>
       <c r="F60" t="s">
-        <v>78</v>
-      </c>
-      <c r="G60" t="s">
-        <v>80</v>
-      </c>
-      <c r="H60" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="G60">
+        <v>202310</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
       </c>
       <c r="I60">
-        <v>202302</v>
+        <v>202.81</v>
       </c>
       <c r="J60">
-        <v>7</v>
-      </c>
-      <c r="K60" t="s">
-        <v>84</v>
+        <v>6</v>
+      </c>
+      <c r="K60">
+        <v>244.68</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -2740,34 +2725,34 @@
         <v>68</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C61" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D61">
-        <v>202301</v>
-      </c>
-      <c r="E61">
-        <v>2</v>
+        <v>202302</v>
+      </c>
+      <c r="E61" t="s">
+        <v>79</v>
       </c>
       <c r="F61" t="s">
-        <v>79</v>
-      </c>
-      <c r="G61" t="s">
-        <v>80</v>
-      </c>
-      <c r="H61" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="G61">
+        <v>202302</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
       </c>
       <c r="I61">
-        <v>202301</v>
+        <v>202.81</v>
       </c>
       <c r="J61">
-        <v>2</v>
-      </c>
-      <c r="K61" t="s">
-        <v>83</v>
+        <v>7</v>
+      </c>
+      <c r="K61">
+        <v>285.46</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -2775,34 +2760,69 @@
         <v>69</v>
       </c>
       <c r="B62" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" t="s">
+        <v>75</v>
+      </c>
+      <c r="D62">
+        <v>202301</v>
+      </c>
+      <c r="E62" t="s">
+        <v>79</v>
+      </c>
+      <c r="F62" t="s">
+        <v>75</v>
+      </c>
+      <c r="G62">
+        <v>202301</v>
+      </c>
+      <c r="H62">
+        <v>2</v>
+      </c>
+      <c r="I62">
+        <v>405.62</v>
+      </c>
+      <c r="J62">
+        <v>2</v>
+      </c>
+      <c r="K62">
+        <v>81.56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" t="s">
         <v>70</v>
       </c>
-      <c r="C62" t="s">
-        <v>71</v>
-      </c>
-      <c r="D62">
-        <v>202310</v>
-      </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62" t="s">
-        <v>78</v>
-      </c>
-      <c r="G62" t="s">
-        <v>80</v>
-      </c>
-      <c r="H62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I62">
-        <v>202310</v>
-      </c>
-      <c r="J62">
-        <v>6</v>
-      </c>
-      <c r="K62" t="s">
-        <v>82</v>
+      <c r="B63" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" t="s">
+        <v>72</v>
+      </c>
+      <c r="D63">
+        <v>202310</v>
+      </c>
+      <c r="E63" t="s">
+        <v>79</v>
+      </c>
+      <c r="F63" t="s">
+        <v>72</v>
+      </c>
+      <c r="G63">
+        <v>202310</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>202.81</v>
+      </c>
+      <c r="J63">
+        <v>6</v>
+      </c>
+      <c r="K63">
+        <v>244.68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>